<commit_message>
Add captain and vice-captain management system - Create scripts to process captain assignments - Merge captains from captain_team_assignments into players file - Pre-assign captains and vice-captains to teams (excluded from auction) - Generate SQL to update Supabase with captain data - Total: 117 players (16 pre-sold, 101 for auction)
</commit_message>
<xml_diff>
--- a/data/CPL_Players_Editable.xlsx
+++ b/data/CPL_Players_Editable.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12504" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,15 +12,17 @@
     <sheet name="Token_Guidelines" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Summary" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Players'!$A$1:$L$95</definedName>
+  </definedNames>
+  <calcPr calcId="191028" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -34,15 +36,35 @@
       <sz val="11"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF252424"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFDDEBF7"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -78,12 +100,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -451,87 +478,107 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L95"/>
+  <dimension ref="A1:P118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.45"/>
   <cols>
     <col width="8" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="32.5546875" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="11.109375" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="14.5546875" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="20.21875" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="21.33203125" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="12.33203125" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="13.5546875" bestFit="1" customWidth="1" min="8" max="8"/>
-    <col width="10.88671875" bestFit="1" customWidth="1" min="9" max="9"/>
-    <col width="26.88671875" bestFit="1" customWidth="1" min="10" max="10"/>
-    <col width="8.33203125" bestFit="1" customWidth="1" min="11" max="11"/>
-    <col width="5.88671875" bestFit="1" customWidth="1" min="12" max="12"/>
+    <col width="32.5703125" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="11.140625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="14.5703125" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="20.28515625" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="21.28515625" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="12.28515625" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="13.5703125" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="10.85546875" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="26.85546875" bestFit="1" customWidth="1" min="10" max="10"/>
+    <col width="8.28515625" bestFit="1" customWidth="1" min="11" max="11"/>
+    <col width="5.85546875" bestFit="1" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>PlayerID</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>EmployeeID</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>ContactNumber</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="5" t="inlineStr">
         <is>
           <t>PreferredRole_Original</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="5" t="inlineStr">
         <is>
           <t>SecondaryRole_Original</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="5" t="inlineStr">
         <is>
           <t>Role</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" s="5" t="inlineStr">
         <is>
           <t>Department</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="I1" s="5" t="inlineStr">
         <is>
           <t>BaseTokens</t>
         </is>
       </c>
-      <c r="J1" s="2" t="inlineStr">
+      <c r="J1" s="5" t="inlineStr">
         <is>
           <t>PhotoFileName</t>
         </is>
       </c>
-      <c r="K1" s="2" t="inlineStr">
+      <c r="K1" s="5" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="L1" s="2" t="inlineStr">
+      <c r="L1" s="5" t="inlineStr">
         <is>
           <t>Notes</t>
+        </is>
+      </c>
+      <c r="M1" s="5" t="inlineStr">
+        <is>
+          <t>IsCaptain</t>
+        </is>
+      </c>
+      <c r="N1" s="5" t="inlineStr">
+        <is>
+          <t>IsViceCaptain</t>
+        </is>
+      </c>
+      <c r="O1" s="5" t="inlineStr">
+        <is>
+          <t>SoldTo</t>
+        </is>
+      </c>
+      <c r="P1" s="5" t="inlineStr">
+        <is>
+          <t>SoldPrice</t>
         </is>
       </c>
     </row>
@@ -588,6 +635,14 @@
         </is>
       </c>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -642,6 +697,14 @@
         </is>
       </c>
       <c r="L3" t="inlineStr"/>
+      <c r="M3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" t="b">
+        <v>0</v>
+      </c>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -696,6 +759,14 @@
         </is>
       </c>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -750,6 +821,14 @@
         </is>
       </c>
       <c r="L5" t="inlineStr"/>
+      <c r="M5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -804,6 +883,14 @@
         </is>
       </c>
       <c r="L6" t="inlineStr"/>
+      <c r="M6" t="b">
+        <v>0</v>
+      </c>
+      <c r="N6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -858,6 +945,14 @@
         </is>
       </c>
       <c r="L7" t="inlineStr"/>
+      <c r="M7" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -908,6 +1003,14 @@
         </is>
       </c>
       <c r="L8" t="inlineStr"/>
+      <c r="M8" t="b">
+        <v>0</v>
+      </c>
+      <c r="N8" t="b">
+        <v>0</v>
+      </c>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -958,6 +1061,14 @@
         </is>
       </c>
       <c r="L9" t="inlineStr"/>
+      <c r="M9" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" t="b">
+        <v>0</v>
+      </c>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1012,6 +1123,14 @@
         </is>
       </c>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10" t="b">
+        <v>0</v>
+      </c>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1066,6 +1185,14 @@
         </is>
       </c>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="b">
+        <v>0</v>
+      </c>
+      <c r="N11" t="b">
+        <v>0</v>
+      </c>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1120,6 +1247,14 @@
         </is>
       </c>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="b">
+        <v>0</v>
+      </c>
+      <c r="N12" t="b">
+        <v>0</v>
+      </c>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1170,6 +1305,14 @@
         </is>
       </c>
       <c r="L13" t="inlineStr"/>
+      <c r="M13" t="b">
+        <v>0</v>
+      </c>
+      <c r="N13" t="b">
+        <v>0</v>
+      </c>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1224,6 +1367,14 @@
         </is>
       </c>
       <c r="L14" t="inlineStr"/>
+      <c r="M14" t="b">
+        <v>0</v>
+      </c>
+      <c r="N14" t="b">
+        <v>0</v>
+      </c>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1278,6 +1429,14 @@
         </is>
       </c>
       <c r="L15" t="inlineStr"/>
+      <c r="M15" t="b">
+        <v>0</v>
+      </c>
+      <c r="N15" t="b">
+        <v>0</v>
+      </c>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1328,6 +1487,14 @@
         </is>
       </c>
       <c r="L16" t="inlineStr"/>
+      <c r="M16" t="b">
+        <v>0</v>
+      </c>
+      <c r="N16" t="b">
+        <v>0</v>
+      </c>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1382,6 +1549,14 @@
         </is>
       </c>
       <c r="L17" t="inlineStr"/>
+      <c r="M17" t="b">
+        <v>0</v>
+      </c>
+      <c r="N17" t="b">
+        <v>0</v>
+      </c>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1414,7 +1589,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Batsman</t>
+          <t>Bowler</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1436,6 +1611,14 @@
         </is>
       </c>
       <c r="L18" t="inlineStr"/>
+      <c r="M18" t="b">
+        <v>0</v>
+      </c>
+      <c r="N18" t="b">
+        <v>0</v>
+      </c>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1468,7 +1651,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Batsman</t>
+          <t>Bowler</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1490,6 +1673,14 @@
         </is>
       </c>
       <c r="L19" t="inlineStr"/>
+      <c r="M19" t="b">
+        <v>0</v>
+      </c>
+      <c r="N19" t="b">
+        <v>0</v>
+      </c>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1544,6 +1735,14 @@
         </is>
       </c>
       <c r="L20" t="inlineStr"/>
+      <c r="M20" t="b">
+        <v>0</v>
+      </c>
+      <c r="N20" t="b">
+        <v>0</v>
+      </c>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1598,6 +1797,14 @@
         </is>
       </c>
       <c r="L21" t="inlineStr"/>
+      <c r="M21" t="b">
+        <v>0</v>
+      </c>
+      <c r="N21" t="b">
+        <v>0</v>
+      </c>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1652,6 +1859,14 @@
         </is>
       </c>
       <c r="L22" t="inlineStr"/>
+      <c r="M22" t="b">
+        <v>0</v>
+      </c>
+      <c r="N22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1684,7 +1899,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Batsman</t>
+          <t>Bowler</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1706,6 +1921,14 @@
         </is>
       </c>
       <c r="L23" t="inlineStr"/>
+      <c r="M23" t="b">
+        <v>0</v>
+      </c>
+      <c r="N23" t="b">
+        <v>0</v>
+      </c>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1760,6 +1983,14 @@
         </is>
       </c>
       <c r="L24" t="inlineStr"/>
+      <c r="M24" t="b">
+        <v>0</v>
+      </c>
+      <c r="N24" t="b">
+        <v>0</v>
+      </c>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1814,6 +2045,14 @@
         </is>
       </c>
       <c r="L25" t="inlineStr"/>
+      <c r="M25" t="b">
+        <v>0</v>
+      </c>
+      <c r="N25" t="b">
+        <v>0</v>
+      </c>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1868,6 +2107,14 @@
         </is>
       </c>
       <c r="L26" t="inlineStr"/>
+      <c r="M26" t="b">
+        <v>0</v>
+      </c>
+      <c r="N26" t="b">
+        <v>0</v>
+      </c>
+      <c r="O26" t="inlineStr"/>
+      <c r="P26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1922,6 +2169,14 @@
         </is>
       </c>
       <c r="L27" t="inlineStr"/>
+      <c r="M27" t="b">
+        <v>0</v>
+      </c>
+      <c r="N27" t="b">
+        <v>0</v>
+      </c>
+      <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1976,6 +2231,14 @@
         </is>
       </c>
       <c r="L28" t="inlineStr"/>
+      <c r="M28" t="b">
+        <v>0</v>
+      </c>
+      <c r="N28" t="b">
+        <v>0</v>
+      </c>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2030,6 +2293,14 @@
         </is>
       </c>
       <c r="L29" t="inlineStr"/>
+      <c r="M29" t="b">
+        <v>0</v>
+      </c>
+      <c r="N29" t="b">
+        <v>0</v>
+      </c>
+      <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2084,6 +2355,14 @@
         </is>
       </c>
       <c r="L30" t="inlineStr"/>
+      <c r="M30" t="b">
+        <v>0</v>
+      </c>
+      <c r="N30" t="b">
+        <v>0</v>
+      </c>
+      <c r="O30" t="inlineStr"/>
+      <c r="P30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2138,6 +2417,14 @@
         </is>
       </c>
       <c r="L31" t="inlineStr"/>
+      <c r="M31" t="b">
+        <v>0</v>
+      </c>
+      <c r="N31" t="b">
+        <v>0</v>
+      </c>
+      <c r="O31" t="inlineStr"/>
+      <c r="P31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2192,6 +2479,14 @@
         </is>
       </c>
       <c r="L32" t="inlineStr"/>
+      <c r="M32" t="b">
+        <v>0</v>
+      </c>
+      <c r="N32" t="b">
+        <v>0</v>
+      </c>
+      <c r="O32" t="inlineStr"/>
+      <c r="P32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2246,6 +2541,14 @@
         </is>
       </c>
       <c r="L33" t="inlineStr"/>
+      <c r="M33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N33" t="b">
+        <v>0</v>
+      </c>
+      <c r="O33" t="inlineStr"/>
+      <c r="P33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2300,6 +2603,14 @@
         </is>
       </c>
       <c r="L34" t="inlineStr"/>
+      <c r="M34" t="b">
+        <v>0</v>
+      </c>
+      <c r="N34" t="b">
+        <v>0</v>
+      </c>
+      <c r="O34" t="inlineStr"/>
+      <c r="P34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2354,6 +2665,14 @@
         </is>
       </c>
       <c r="L35" t="inlineStr"/>
+      <c r="M35" t="b">
+        <v>0</v>
+      </c>
+      <c r="N35" t="b">
+        <v>0</v>
+      </c>
+      <c r="O35" t="inlineStr"/>
+      <c r="P35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2404,6 +2723,14 @@
         </is>
       </c>
       <c r="L36" t="inlineStr"/>
+      <c r="M36" t="b">
+        <v>0</v>
+      </c>
+      <c r="N36" t="b">
+        <v>0</v>
+      </c>
+      <c r="O36" t="inlineStr"/>
+      <c r="P36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2458,6 +2785,14 @@
         </is>
       </c>
       <c r="L37" t="inlineStr"/>
+      <c r="M37" t="b">
+        <v>0</v>
+      </c>
+      <c r="N37" t="b">
+        <v>0</v>
+      </c>
+      <c r="O37" t="inlineStr"/>
+      <c r="P37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2512,6 +2847,14 @@
         </is>
       </c>
       <c r="L38" t="inlineStr"/>
+      <c r="M38" t="b">
+        <v>0</v>
+      </c>
+      <c r="N38" t="b">
+        <v>0</v>
+      </c>
+      <c r="O38" t="inlineStr"/>
+      <c r="P38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2562,6 +2905,14 @@
         </is>
       </c>
       <c r="L39" t="inlineStr"/>
+      <c r="M39" t="b">
+        <v>0</v>
+      </c>
+      <c r="N39" t="b">
+        <v>0</v>
+      </c>
+      <c r="O39" t="inlineStr"/>
+      <c r="P39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2594,7 +2945,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>All-rounder</t>
+          <t>Bowler</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -2616,6 +2967,14 @@
         </is>
       </c>
       <c r="L40" t="inlineStr"/>
+      <c r="M40" t="b">
+        <v>0</v>
+      </c>
+      <c r="N40" t="b">
+        <v>0</v>
+      </c>
+      <c r="O40" t="inlineStr"/>
+      <c r="P40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2670,6 +3029,14 @@
         </is>
       </c>
       <c r="L41" t="inlineStr"/>
+      <c r="M41" t="b">
+        <v>0</v>
+      </c>
+      <c r="N41" t="b">
+        <v>0</v>
+      </c>
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2720,6 +3087,14 @@
         </is>
       </c>
       <c r="L42" t="inlineStr"/>
+      <c r="M42" t="b">
+        <v>0</v>
+      </c>
+      <c r="N42" t="b">
+        <v>0</v>
+      </c>
+      <c r="O42" t="inlineStr"/>
+      <c r="P42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2752,7 +3127,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>All-rounder</t>
+          <t>Bowler</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -2774,6 +3149,14 @@
         </is>
       </c>
       <c r="L43" t="inlineStr"/>
+      <c r="M43" t="b">
+        <v>0</v>
+      </c>
+      <c r="N43" t="b">
+        <v>0</v>
+      </c>
+      <c r="O43" t="inlineStr"/>
+      <c r="P43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2824,6 +3207,14 @@
         </is>
       </c>
       <c r="L44" t="inlineStr"/>
+      <c r="M44" t="b">
+        <v>0</v>
+      </c>
+      <c r="N44" t="b">
+        <v>0</v>
+      </c>
+      <c r="O44" t="inlineStr"/>
+      <c r="P44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2856,7 +3247,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>All-rounder</t>
+          <t>Bowler</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -2878,6 +3269,14 @@
         </is>
       </c>
       <c r="L45" t="inlineStr"/>
+      <c r="M45" t="b">
+        <v>0</v>
+      </c>
+      <c r="N45" t="b">
+        <v>0</v>
+      </c>
+      <c r="O45" t="inlineStr"/>
+      <c r="P45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2932,6 +3331,14 @@
         </is>
       </c>
       <c r="L46" t="inlineStr"/>
+      <c r="M46" t="b">
+        <v>0</v>
+      </c>
+      <c r="N46" t="b">
+        <v>0</v>
+      </c>
+      <c r="O46" t="inlineStr"/>
+      <c r="P46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2964,7 +3371,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>All-rounder</t>
+          <t>Bowler</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -2986,6 +3393,14 @@
         </is>
       </c>
       <c r="L47" t="inlineStr"/>
+      <c r="M47" t="b">
+        <v>0</v>
+      </c>
+      <c r="N47" t="b">
+        <v>0</v>
+      </c>
+      <c r="O47" t="inlineStr"/>
+      <c r="P47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -3036,6 +3451,14 @@
         </is>
       </c>
       <c r="L48" t="inlineStr"/>
+      <c r="M48" t="b">
+        <v>0</v>
+      </c>
+      <c r="N48" t="b">
+        <v>0</v>
+      </c>
+      <c r="O48" t="inlineStr"/>
+      <c r="P48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -3068,7 +3491,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>All-rounder</t>
+          <t>Bowler</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -3090,6 +3513,14 @@
         </is>
       </c>
       <c r="L49" t="inlineStr"/>
+      <c r="M49" t="b">
+        <v>0</v>
+      </c>
+      <c r="N49" t="b">
+        <v>0</v>
+      </c>
+      <c r="O49" t="inlineStr"/>
+      <c r="P49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -3144,6 +3575,14 @@
         </is>
       </c>
       <c r="L50" t="inlineStr"/>
+      <c r="M50" t="b">
+        <v>0</v>
+      </c>
+      <c r="N50" t="b">
+        <v>0</v>
+      </c>
+      <c r="O50" t="inlineStr"/>
+      <c r="P50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -3198,6 +3637,14 @@
         </is>
       </c>
       <c r="L51" t="inlineStr"/>
+      <c r="M51" t="b">
+        <v>0</v>
+      </c>
+      <c r="N51" t="b">
+        <v>0</v>
+      </c>
+      <c r="O51" t="inlineStr"/>
+      <c r="P51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -3252,6 +3699,14 @@
         </is>
       </c>
       <c r="L52" t="inlineStr"/>
+      <c r="M52" t="b">
+        <v>0</v>
+      </c>
+      <c r="N52" t="b">
+        <v>0</v>
+      </c>
+      <c r="O52" t="inlineStr"/>
+      <c r="P52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -3306,6 +3761,14 @@
         </is>
       </c>
       <c r="L53" t="inlineStr"/>
+      <c r="M53" t="b">
+        <v>0</v>
+      </c>
+      <c r="N53" t="b">
+        <v>0</v>
+      </c>
+      <c r="O53" t="inlineStr"/>
+      <c r="P53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -3360,6 +3823,14 @@
         </is>
       </c>
       <c r="L54" t="inlineStr"/>
+      <c r="M54" t="b">
+        <v>0</v>
+      </c>
+      <c r="N54" t="b">
+        <v>0</v>
+      </c>
+      <c r="O54" t="inlineStr"/>
+      <c r="P54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -3414,6 +3885,14 @@
         </is>
       </c>
       <c r="L55" t="inlineStr"/>
+      <c r="M55" t="b">
+        <v>0</v>
+      </c>
+      <c r="N55" t="b">
+        <v>0</v>
+      </c>
+      <c r="O55" t="inlineStr"/>
+      <c r="P55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -3468,6 +3947,14 @@
         </is>
       </c>
       <c r="L56" t="inlineStr"/>
+      <c r="M56" t="b">
+        <v>0</v>
+      </c>
+      <c r="N56" t="b">
+        <v>0</v>
+      </c>
+      <c r="O56" t="inlineStr"/>
+      <c r="P56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -3522,6 +4009,14 @@
         </is>
       </c>
       <c r="L57" t="inlineStr"/>
+      <c r="M57" t="b">
+        <v>0</v>
+      </c>
+      <c r="N57" t="b">
+        <v>0</v>
+      </c>
+      <c r="O57" t="inlineStr"/>
+      <c r="P57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -3554,7 +4049,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>All-rounder</t>
+          <t>Bowler</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
@@ -3576,6 +4071,14 @@
         </is>
       </c>
       <c r="L58" t="inlineStr"/>
+      <c r="M58" t="b">
+        <v>0</v>
+      </c>
+      <c r="N58" t="b">
+        <v>0</v>
+      </c>
+      <c r="O58" t="inlineStr"/>
+      <c r="P58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -3630,6 +4133,14 @@
         </is>
       </c>
       <c r="L59" t="inlineStr"/>
+      <c r="M59" t="b">
+        <v>0</v>
+      </c>
+      <c r="N59" t="b">
+        <v>0</v>
+      </c>
+      <c r="O59" t="inlineStr"/>
+      <c r="P59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -3662,7 +4173,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>All-rounder</t>
+          <t>Bowler</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
@@ -3684,6 +4195,14 @@
         </is>
       </c>
       <c r="L60" t="inlineStr"/>
+      <c r="M60" t="b">
+        <v>0</v>
+      </c>
+      <c r="N60" t="b">
+        <v>0</v>
+      </c>
+      <c r="O60" t="inlineStr"/>
+      <c r="P60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -3738,6 +4257,14 @@
         </is>
       </c>
       <c r="L61" t="inlineStr"/>
+      <c r="M61" t="b">
+        <v>0</v>
+      </c>
+      <c r="N61" t="b">
+        <v>0</v>
+      </c>
+      <c r="O61" t="inlineStr"/>
+      <c r="P61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -3792,6 +4319,14 @@
         </is>
       </c>
       <c r="L62" t="inlineStr"/>
+      <c r="M62" t="b">
+        <v>0</v>
+      </c>
+      <c r="N62" t="b">
+        <v>0</v>
+      </c>
+      <c r="O62" t="inlineStr"/>
+      <c r="P62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -3846,6 +4381,14 @@
         </is>
       </c>
       <c r="L63" t="inlineStr"/>
+      <c r="M63" t="b">
+        <v>0</v>
+      </c>
+      <c r="N63" t="b">
+        <v>0</v>
+      </c>
+      <c r="O63" t="inlineStr"/>
+      <c r="P63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -3900,6 +4443,14 @@
         </is>
       </c>
       <c r="L64" t="inlineStr"/>
+      <c r="M64" t="b">
+        <v>0</v>
+      </c>
+      <c r="N64" t="b">
+        <v>0</v>
+      </c>
+      <c r="O64" t="inlineStr"/>
+      <c r="P64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -3954,6 +4505,14 @@
         </is>
       </c>
       <c r="L65" t="inlineStr"/>
+      <c r="M65" t="b">
+        <v>0</v>
+      </c>
+      <c r="N65" t="b">
+        <v>0</v>
+      </c>
+      <c r="O65" t="inlineStr"/>
+      <c r="P65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -3986,7 +4545,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>All-rounder</t>
+          <t>Bowler</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
@@ -4008,6 +4567,14 @@
         </is>
       </c>
       <c r="L66" t="inlineStr"/>
+      <c r="M66" t="b">
+        <v>0</v>
+      </c>
+      <c r="N66" t="b">
+        <v>0</v>
+      </c>
+      <c r="O66" t="inlineStr"/>
+      <c r="P66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -4040,7 +4607,7 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>All-rounder</t>
+          <t>Bowler</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
@@ -4062,6 +4629,14 @@
         </is>
       </c>
       <c r="L67" t="inlineStr"/>
+      <c r="M67" t="b">
+        <v>0</v>
+      </c>
+      <c r="N67" t="b">
+        <v>0</v>
+      </c>
+      <c r="O67" t="inlineStr"/>
+      <c r="P67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -4116,6 +4691,14 @@
         </is>
       </c>
       <c r="L68" t="inlineStr"/>
+      <c r="M68" t="b">
+        <v>0</v>
+      </c>
+      <c r="N68" t="b">
+        <v>0</v>
+      </c>
+      <c r="O68" t="inlineStr"/>
+      <c r="P68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -4170,6 +4753,14 @@
         </is>
       </c>
       <c r="L69" t="inlineStr"/>
+      <c r="M69" t="b">
+        <v>0</v>
+      </c>
+      <c r="N69" t="b">
+        <v>0</v>
+      </c>
+      <c r="O69" t="inlineStr"/>
+      <c r="P69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -4224,6 +4815,14 @@
         </is>
       </c>
       <c r="L70" t="inlineStr"/>
+      <c r="M70" t="b">
+        <v>0</v>
+      </c>
+      <c r="N70" t="b">
+        <v>0</v>
+      </c>
+      <c r="O70" t="inlineStr"/>
+      <c r="P70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -4278,6 +4877,14 @@
         </is>
       </c>
       <c r="L71" t="inlineStr"/>
+      <c r="M71" t="b">
+        <v>0</v>
+      </c>
+      <c r="N71" t="b">
+        <v>0</v>
+      </c>
+      <c r="O71" t="inlineStr"/>
+      <c r="P71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -4332,6 +4939,14 @@
         </is>
       </c>
       <c r="L72" t="inlineStr"/>
+      <c r="M72" t="b">
+        <v>0</v>
+      </c>
+      <c r="N72" t="b">
+        <v>0</v>
+      </c>
+      <c r="O72" t="inlineStr"/>
+      <c r="P72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -4386,6 +5001,14 @@
         </is>
       </c>
       <c r="L73" t="inlineStr"/>
+      <c r="M73" t="b">
+        <v>0</v>
+      </c>
+      <c r="N73" t="b">
+        <v>0</v>
+      </c>
+      <c r="O73" t="inlineStr"/>
+      <c r="P73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -4418,7 +5041,7 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>All-rounder</t>
+          <t>Bowler</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
@@ -4440,6 +5063,14 @@
         </is>
       </c>
       <c r="L74" t="inlineStr"/>
+      <c r="M74" t="b">
+        <v>0</v>
+      </c>
+      <c r="N74" t="b">
+        <v>0</v>
+      </c>
+      <c r="O74" t="inlineStr"/>
+      <c r="P74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -4490,6 +5121,14 @@
         </is>
       </c>
       <c r="L75" t="inlineStr"/>
+      <c r="M75" t="b">
+        <v>0</v>
+      </c>
+      <c r="N75" t="b">
+        <v>0</v>
+      </c>
+      <c r="O75" t="inlineStr"/>
+      <c r="P75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -4522,7 +5161,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>All-rounder</t>
+          <t>Bowler</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
@@ -4544,6 +5183,14 @@
         </is>
       </c>
       <c r="L76" t="inlineStr"/>
+      <c r="M76" t="b">
+        <v>0</v>
+      </c>
+      <c r="N76" t="b">
+        <v>0</v>
+      </c>
+      <c r="O76" t="inlineStr"/>
+      <c r="P76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -4572,7 +5219,7 @@
       <c r="F77" t="inlineStr"/>
       <c r="G77" t="inlineStr">
         <is>
-          <t>All-rounder</t>
+          <t>Bowler</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
@@ -4594,6 +5241,14 @@
         </is>
       </c>
       <c r="L77" t="inlineStr"/>
+      <c r="M77" t="b">
+        <v>0</v>
+      </c>
+      <c r="N77" t="b">
+        <v>0</v>
+      </c>
+      <c r="O77" t="inlineStr"/>
+      <c r="P77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -4648,6 +5303,14 @@
         </is>
       </c>
       <c r="L78" t="inlineStr"/>
+      <c r="M78" t="b">
+        <v>0</v>
+      </c>
+      <c r="N78" t="b">
+        <v>0</v>
+      </c>
+      <c r="O78" t="inlineStr"/>
+      <c r="P78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -4702,6 +5365,14 @@
         </is>
       </c>
       <c r="L79" t="inlineStr"/>
+      <c r="M79" t="b">
+        <v>0</v>
+      </c>
+      <c r="N79" t="b">
+        <v>0</v>
+      </c>
+      <c r="O79" t="inlineStr"/>
+      <c r="P79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -4730,7 +5401,7 @@
       <c r="F80" t="inlineStr"/>
       <c r="G80" t="inlineStr">
         <is>
-          <t>All-rounder</t>
+          <t>Bowler</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
@@ -4752,6 +5423,14 @@
         </is>
       </c>
       <c r="L80" t="inlineStr"/>
+      <c r="M80" t="b">
+        <v>0</v>
+      </c>
+      <c r="N80" t="b">
+        <v>0</v>
+      </c>
+      <c r="O80" t="inlineStr"/>
+      <c r="P80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -4806,6 +5485,14 @@
         </is>
       </c>
       <c r="L81" t="inlineStr"/>
+      <c r="M81" t="b">
+        <v>0</v>
+      </c>
+      <c r="N81" t="b">
+        <v>0</v>
+      </c>
+      <c r="O81" t="inlineStr"/>
+      <c r="P81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -4860,6 +5547,14 @@
         </is>
       </c>
       <c r="L82" t="inlineStr"/>
+      <c r="M82" t="b">
+        <v>0</v>
+      </c>
+      <c r="N82" t="b">
+        <v>0</v>
+      </c>
+      <c r="O82" t="inlineStr"/>
+      <c r="P82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -4914,6 +5609,14 @@
         </is>
       </c>
       <c r="L83" t="inlineStr"/>
+      <c r="M83" t="b">
+        <v>0</v>
+      </c>
+      <c r="N83" t="b">
+        <v>0</v>
+      </c>
+      <c r="O83" t="inlineStr"/>
+      <c r="P83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -4968,6 +5671,14 @@
         </is>
       </c>
       <c r="L84" t="inlineStr"/>
+      <c r="M84" t="b">
+        <v>0</v>
+      </c>
+      <c r="N84" t="b">
+        <v>0</v>
+      </c>
+      <c r="O84" t="inlineStr"/>
+      <c r="P84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -5022,6 +5733,14 @@
         </is>
       </c>
       <c r="L85" t="inlineStr"/>
+      <c r="M85" t="b">
+        <v>0</v>
+      </c>
+      <c r="N85" t="b">
+        <v>0</v>
+      </c>
+      <c r="O85" t="inlineStr"/>
+      <c r="P85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -5076,6 +5795,14 @@
         </is>
       </c>
       <c r="L86" t="inlineStr"/>
+      <c r="M86" t="b">
+        <v>0</v>
+      </c>
+      <c r="N86" t="b">
+        <v>0</v>
+      </c>
+      <c r="O86" t="inlineStr"/>
+      <c r="P86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -5130,6 +5857,14 @@
         </is>
       </c>
       <c r="L87" t="inlineStr"/>
+      <c r="M87" t="b">
+        <v>0</v>
+      </c>
+      <c r="N87" t="b">
+        <v>0</v>
+      </c>
+      <c r="O87" t="inlineStr"/>
+      <c r="P87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -5184,6 +5919,14 @@
         </is>
       </c>
       <c r="L88" t="inlineStr"/>
+      <c r="M88" t="b">
+        <v>0</v>
+      </c>
+      <c r="N88" t="b">
+        <v>0</v>
+      </c>
+      <c r="O88" t="inlineStr"/>
+      <c r="P88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -5238,6 +5981,14 @@
         </is>
       </c>
       <c r="L89" t="inlineStr"/>
+      <c r="M89" t="b">
+        <v>0</v>
+      </c>
+      <c r="N89" t="b">
+        <v>0</v>
+      </c>
+      <c r="O89" t="inlineStr"/>
+      <c r="P89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -5292,6 +6043,14 @@
         </is>
       </c>
       <c r="L90" t="inlineStr"/>
+      <c r="M90" t="b">
+        <v>0</v>
+      </c>
+      <c r="N90" t="b">
+        <v>0</v>
+      </c>
+      <c r="O90" t="inlineStr"/>
+      <c r="P90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -5346,6 +6105,14 @@
         </is>
       </c>
       <c r="L91" t="inlineStr"/>
+      <c r="M91" t="b">
+        <v>0</v>
+      </c>
+      <c r="N91" t="b">
+        <v>0</v>
+      </c>
+      <c r="O91" t="inlineStr"/>
+      <c r="P91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -5400,6 +6167,14 @@
         </is>
       </c>
       <c r="L92" t="inlineStr"/>
+      <c r="M92" t="b">
+        <v>0</v>
+      </c>
+      <c r="N92" t="b">
+        <v>0</v>
+      </c>
+      <c r="O92" t="inlineStr"/>
+      <c r="P92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -5454,6 +6229,14 @@
         </is>
       </c>
       <c r="L93" t="inlineStr"/>
+      <c r="M93" t="b">
+        <v>0</v>
+      </c>
+      <c r="N93" t="b">
+        <v>0</v>
+      </c>
+      <c r="O93" t="inlineStr"/>
+      <c r="P93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -5508,6 +6291,14 @@
         </is>
       </c>
       <c r="L94" t="inlineStr"/>
+      <c r="M94" t="b">
+        <v>0</v>
+      </c>
+      <c r="N94" t="b">
+        <v>0</v>
+      </c>
+      <c r="O94" t="inlineStr"/>
+      <c r="P94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -5562,8 +6353,1219 @@
         </is>
       </c>
       <c r="L95" t="inlineStr"/>
+      <c r="M95" t="b">
+        <v>0</v>
+      </c>
+      <c r="N95" t="b">
+        <v>0</v>
+      </c>
+      <c r="O95" t="inlineStr"/>
+      <c r="P95" t="inlineStr"/>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>7THE</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Jaidev Beniwal</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>7THE</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>9989153796</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Batsman</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>Bowler</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>Batsman</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>Batting</t>
+        </is>
+      </c>
+      <c r="I96" t="n">
+        <v>35</v>
+      </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>7THE.jpg</t>
+        </is>
+      </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="L96" t="inlineStr"/>
+      <c r="M96" t="b">
+        <v>0</v>
+      </c>
+      <c r="N96" t="b">
+        <v>0</v>
+      </c>
+      <c r="O96" t="inlineStr"/>
+      <c r="P96" t="inlineStr"/>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>304A</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Shubham Kumar Jena</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>304A</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>7032441363</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Batting All-rounder</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>Bowler</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>All-rounder</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>All-rounder</t>
+        </is>
+      </c>
+      <c r="I97" t="n">
+        <v>40</v>
+      </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>304A.jpg</t>
+        </is>
+      </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="L97" t="inlineStr"/>
+      <c r="M97" t="b">
+        <v>0</v>
+      </c>
+      <c r="N97" t="b">
+        <v>0</v>
+      </c>
+      <c r="O97" t="inlineStr"/>
+      <c r="P97" t="inlineStr"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="inlineStr">
+        <is>
+          <t>917V</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Bharath Chaitanya Jagana</t>
+        </is>
+      </c>
+      <c r="C98" s="2" t="inlineStr">
+        <is>
+          <t>917V</t>
+        </is>
+      </c>
+      <c r="D98" s="3" t="n">
+        <v>7288959841</v>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Bowling All-rounder</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>Batting</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>Bowler</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>All-rounder</t>
+        </is>
+      </c>
+      <c r="I98" t="n">
+        <v>40</v>
+      </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>917V.jpg</t>
+        </is>
+      </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="L98" t="inlineStr"/>
+      <c r="M98" t="b">
+        <v>0</v>
+      </c>
+      <c r="N98" t="b">
+        <v>0</v>
+      </c>
+      <c r="O98" t="inlineStr"/>
+      <c r="P98" t="inlineStr"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="2" t="inlineStr">
+        <is>
+          <t>7CFH</t>
+        </is>
+      </c>
+      <c r="B99" s="1" t="inlineStr">
+        <is>
+          <t>Priyank Kumar Babburu</t>
+        </is>
+      </c>
+      <c r="C99" s="2" t="inlineStr">
+        <is>
+          <t>7CFH</t>
+        </is>
+      </c>
+      <c r="D99" s="2" t="n">
+        <v>9966557977</v>
+      </c>
+      <c r="E99" s="2" t="inlineStr">
+        <is>
+          <t>Batting All-rounder</t>
+        </is>
+      </c>
+      <c r="F99" s="2" t="inlineStr">
+        <is>
+          <t>Bowler</t>
+        </is>
+      </c>
+      <c r="G99" s="2" t="inlineStr">
+        <is>
+          <t>Batsman</t>
+        </is>
+      </c>
+      <c r="H99" s="2" t="inlineStr">
+        <is>
+          <t>Batting</t>
+        </is>
+      </c>
+      <c r="I99" t="n">
+        <v>35</v>
+      </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t>7CFH.jpg</t>
+        </is>
+      </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="L99" t="inlineStr"/>
+      <c r="M99" t="b">
+        <v>0</v>
+      </c>
+      <c r="N99" t="b">
+        <v>0</v>
+      </c>
+      <c r="O99" t="inlineStr"/>
+      <c r="P99" t="inlineStr"/>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>5DXX</t>
+        </is>
+      </c>
+      <c r="B100" s="1" t="inlineStr">
+        <is>
+          <t>Siva Naga Kishore Raju Samanthapudi</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>5DXX</t>
+        </is>
+      </c>
+      <c r="D100" s="2" t="n">
+        <v>9866414485</v>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Batsman</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>Wicket Keeper</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>WicketKeeper</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>Wicket Keeping</t>
+        </is>
+      </c>
+      <c r="I100" t="n">
+        <v>35</v>
+      </c>
+      <c r="J100" t="inlineStr">
+        <is>
+          <t>5DXX.jpg</t>
+        </is>
+      </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="L100" t="inlineStr"/>
+      <c r="M100" t="b">
+        <v>0</v>
+      </c>
+      <c r="N100" t="b">
+        <v>0</v>
+      </c>
+      <c r="O100" t="inlineStr"/>
+      <c r="P100" t="inlineStr"/>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>14HB</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Mahether Reddy Bhavanam</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr"/>
+      <c r="D101" t="inlineStr"/>
+      <c r="E101" t="inlineStr"/>
+      <c r="F101" t="inlineStr"/>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>WicketKeeper</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr"/>
+      <c r="I101" t="n">
+        <v>45</v>
+      </c>
+      <c r="J101" t="inlineStr">
+        <is>
+          <t>14HB.jpg</t>
+        </is>
+      </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>Sold</t>
+        </is>
+      </c>
+      <c r="L101" t="inlineStr"/>
+      <c r="M101" t="b">
+        <v>0</v>
+      </c>
+      <c r="N101" t="b">
+        <v>0</v>
+      </c>
+      <c r="O101" t="inlineStr">
+        <is>
+          <t>Team 1</t>
+        </is>
+      </c>
+      <c r="P101" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>44QM</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Niranjan Reddy Midde</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr"/>
+      <c r="D102" t="inlineStr"/>
+      <c r="E102" t="inlineStr"/>
+      <c r="F102" t="inlineStr"/>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>All-rounder</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr"/>
+      <c r="I102" t="n">
+        <v>50</v>
+      </c>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t>44QM.jpg</t>
+        </is>
+      </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>Sold</t>
+        </is>
+      </c>
+      <c r="L102" t="inlineStr"/>
+      <c r="M102" t="b">
+        <v>0</v>
+      </c>
+      <c r="N102" t="b">
+        <v>1</v>
+      </c>
+      <c r="O102" t="inlineStr">
+        <is>
+          <t>Team 5</t>
+        </is>
+      </c>
+      <c r="P102" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>628B</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Jagadish Babu Koppula Venkata</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr"/>
+      <c r="D103" t="inlineStr"/>
+      <c r="E103" t="inlineStr"/>
+      <c r="F103" t="inlineStr"/>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>All-rounder</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr"/>
+      <c r="I103" t="n">
+        <v>50</v>
+      </c>
+      <c r="J103" t="inlineStr">
+        <is>
+          <t>628B.jpg</t>
+        </is>
+      </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>Sold</t>
+        </is>
+      </c>
+      <c r="L103" t="inlineStr"/>
+      <c r="M103" t="b">
+        <v>1</v>
+      </c>
+      <c r="N103" t="b">
+        <v>0</v>
+      </c>
+      <c r="O103" t="inlineStr">
+        <is>
+          <t>Team 6</t>
+        </is>
+      </c>
+      <c r="P103" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>6NN4</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Rajasekhara Reddy Gowkanapalli</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr"/>
+      <c r="D104" t="inlineStr"/>
+      <c r="E104" t="inlineStr"/>
+      <c r="F104" t="inlineStr"/>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>All-rounder</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr"/>
+      <c r="I104" t="n">
+        <v>50</v>
+      </c>
+      <c r="J104" t="inlineStr">
+        <is>
+          <t>6NN4.jpg</t>
+        </is>
+      </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>Sold</t>
+        </is>
+      </c>
+      <c r="L104" t="inlineStr"/>
+      <c r="M104" t="b">
+        <v>0</v>
+      </c>
+      <c r="N104" t="b">
+        <v>1</v>
+      </c>
+      <c r="O104" t="inlineStr">
+        <is>
+          <t>Team 7</t>
+        </is>
+      </c>
+      <c r="P104" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>4V2H</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Debargha Gupta</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr"/>
+      <c r="D105" t="inlineStr"/>
+      <c r="E105" t="inlineStr"/>
+      <c r="F105" t="inlineStr"/>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>All-rounder</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr"/>
+      <c r="I105" t="n">
+        <v>50</v>
+      </c>
+      <c r="J105" t="inlineStr">
+        <is>
+          <t>4V2H.jpg</t>
+        </is>
+      </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>Sold</t>
+        </is>
+      </c>
+      <c r="L105" t="inlineStr"/>
+      <c r="M105" t="b">
+        <v>0</v>
+      </c>
+      <c r="N105" t="b">
+        <v>1</v>
+      </c>
+      <c r="O105" t="inlineStr">
+        <is>
+          <t>Team 1</t>
+        </is>
+      </c>
+      <c r="P105" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2BJB</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Pradeep Kumar Pala</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr"/>
+      <c r="D106" t="inlineStr"/>
+      <c r="E106" t="inlineStr"/>
+      <c r="F106" t="inlineStr"/>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>All-rounder</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr"/>
+      <c r="I106" t="n">
+        <v>50</v>
+      </c>
+      <c r="J106" t="inlineStr">
+        <is>
+          <t>2BJB.jpg</t>
+        </is>
+      </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>Sold</t>
+        </is>
+      </c>
+      <c r="L106" t="inlineStr"/>
+      <c r="M106" t="b">
+        <v>1</v>
+      </c>
+      <c r="N106" t="b">
+        <v>0</v>
+      </c>
+      <c r="O106" t="inlineStr">
+        <is>
+          <t>Team 4</t>
+        </is>
+      </c>
+      <c r="P106" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>615R</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Siva Teja Pidikiti</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr"/>
+      <c r="D107" t="inlineStr"/>
+      <c r="E107" t="inlineStr"/>
+      <c r="F107" t="inlineStr"/>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>All-rounder</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr"/>
+      <c r="I107" t="n">
+        <v>50</v>
+      </c>
+      <c r="J107" t="inlineStr">
+        <is>
+          <t>615R.jpg</t>
+        </is>
+      </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>Sold</t>
+        </is>
+      </c>
+      <c r="L107" t="inlineStr"/>
+      <c r="M107" t="b">
+        <v>1</v>
+      </c>
+      <c r="N107" t="b">
+        <v>0</v>
+      </c>
+      <c r="O107" t="inlineStr">
+        <is>
+          <t>Team 5</t>
+        </is>
+      </c>
+      <c r="P107" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>5K5T</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Abdul Sohail Mohammed</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr"/>
+      <c r="D108" t="inlineStr"/>
+      <c r="E108" t="inlineStr"/>
+      <c r="F108" t="inlineStr"/>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>All-rounder</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr"/>
+      <c r="I108" t="n">
+        <v>50</v>
+      </c>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>5K5T.jpg</t>
+        </is>
+      </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>Sold</t>
+        </is>
+      </c>
+      <c r="L108" t="inlineStr"/>
+      <c r="M108" t="b">
+        <v>0</v>
+      </c>
+      <c r="N108" t="b">
+        <v>1</v>
+      </c>
+      <c r="O108" t="inlineStr">
+        <is>
+          <t>Team 4</t>
+        </is>
+      </c>
+      <c r="P108" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>4FF3</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Dinesh Palem</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr"/>
+      <c r="D109" t="inlineStr"/>
+      <c r="E109" t="inlineStr"/>
+      <c r="F109" t="inlineStr"/>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>WicketKeeper</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr"/>
+      <c r="I109" t="n">
+        <v>45</v>
+      </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>4FF3.jpg</t>
+        </is>
+      </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>Sold</t>
+        </is>
+      </c>
+      <c r="L109" t="inlineStr"/>
+      <c r="M109" t="b">
+        <v>0</v>
+      </c>
+      <c r="N109" t="b">
+        <v>1</v>
+      </c>
+      <c r="O109" t="inlineStr">
+        <is>
+          <t>Team 2</t>
+        </is>
+      </c>
+      <c r="P109" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>PVF0</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Srikanth Jaina</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr"/>
+      <c r="D110" t="inlineStr"/>
+      <c r="E110" t="inlineStr"/>
+      <c r="F110" t="inlineStr"/>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>Batsman</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr"/>
+      <c r="I110" t="n">
+        <v>45</v>
+      </c>
+      <c r="J110" t="inlineStr">
+        <is>
+          <t>PVF0.jpg</t>
+        </is>
+      </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="L110" t="inlineStr"/>
+      <c r="M110" t="b">
+        <v>0</v>
+      </c>
+      <c r="N110" t="b">
+        <v>0</v>
+      </c>
+      <c r="O110" t="inlineStr"/>
+      <c r="P110" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>MXL5</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Anil Maradani</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr"/>
+      <c r="D111" t="inlineStr"/>
+      <c r="E111" t="inlineStr"/>
+      <c r="F111" t="inlineStr"/>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>Batsman</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr"/>
+      <c r="I111" t="n">
+        <v>45</v>
+      </c>
+      <c r="J111" t="inlineStr">
+        <is>
+          <t>MXL5.jpg</t>
+        </is>
+      </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>Sold</t>
+        </is>
+      </c>
+      <c r="L111" t="inlineStr"/>
+      <c r="M111" t="b">
+        <v>0</v>
+      </c>
+      <c r="N111" t="b">
+        <v>0</v>
+      </c>
+      <c r="O111" t="inlineStr">
+        <is>
+          <t>Team 2</t>
+        </is>
+      </c>
+      <c r="P111" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>7B8V</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Saravanan Krishnamoorthy</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr"/>
+      <c r="D112" t="inlineStr"/>
+      <c r="E112" t="inlineStr"/>
+      <c r="F112" t="inlineStr"/>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>All-rounder</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr"/>
+      <c r="I112" t="n">
+        <v>50</v>
+      </c>
+      <c r="J112" t="inlineStr">
+        <is>
+          <t>7B8V.jpg</t>
+        </is>
+      </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>Sold</t>
+        </is>
+      </c>
+      <c r="L112" t="inlineStr"/>
+      <c r="M112" t="b">
+        <v>1</v>
+      </c>
+      <c r="N112" t="b">
+        <v>0</v>
+      </c>
+      <c r="O112" t="inlineStr">
+        <is>
+          <t>Team 8</t>
+        </is>
+      </c>
+      <c r="P112" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>5CLA</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Gopi Krishna Kanth Dabbakuti</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr"/>
+      <c r="D113" t="inlineStr"/>
+      <c r="E113" t="inlineStr"/>
+      <c r="F113" t="inlineStr"/>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>All-rounder</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr"/>
+      <c r="I113" t="n">
+        <v>50</v>
+      </c>
+      <c r="J113" t="inlineStr">
+        <is>
+          <t>5CLA.jpg</t>
+        </is>
+      </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>Sold</t>
+        </is>
+      </c>
+      <c r="L113" t="inlineStr"/>
+      <c r="M113" t="b">
+        <v>0</v>
+      </c>
+      <c r="N113" t="b">
+        <v>1</v>
+      </c>
+      <c r="O113" t="inlineStr">
+        <is>
+          <t>Team 3</t>
+        </is>
+      </c>
+      <c r="P113" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>6RMT</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Veera Venkata Naga Satya Raj Gollapalli</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr"/>
+      <c r="D114" t="inlineStr"/>
+      <c r="E114" t="inlineStr"/>
+      <c r="F114" t="inlineStr"/>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>All-rounder</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr"/>
+      <c r="I114" t="n">
+        <v>50</v>
+      </c>
+      <c r="J114" t="inlineStr">
+        <is>
+          <t>6RMT.jpg</t>
+        </is>
+      </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>Sold</t>
+        </is>
+      </c>
+      <c r="L114" t="inlineStr"/>
+      <c r="M114" t="b">
+        <v>0</v>
+      </c>
+      <c r="N114" t="b">
+        <v>1</v>
+      </c>
+      <c r="O114" t="inlineStr">
+        <is>
+          <t>Team 6</t>
+        </is>
+      </c>
+      <c r="P114" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>53JX</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Sairam Singh Balaji</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr"/>
+      <c r="D115" t="inlineStr"/>
+      <c r="E115" t="inlineStr"/>
+      <c r="F115" t="inlineStr"/>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>WicketKeeper</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr"/>
+      <c r="I115" t="n">
+        <v>45</v>
+      </c>
+      <c r="J115" t="inlineStr">
+        <is>
+          <t>53JX.jpg</t>
+        </is>
+      </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>Sold</t>
+        </is>
+      </c>
+      <c r="L115" t="inlineStr"/>
+      <c r="M115" t="b">
+        <v>1</v>
+      </c>
+      <c r="N115" t="b">
+        <v>0</v>
+      </c>
+      <c r="O115" t="inlineStr">
+        <is>
+          <t>Team 7</t>
+        </is>
+      </c>
+      <c r="P115" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>8E1D</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Mahesh Gaada</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr"/>
+      <c r="D116" t="inlineStr"/>
+      <c r="E116" t="inlineStr"/>
+      <c r="F116" t="inlineStr"/>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>WicketKeeper</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr"/>
+      <c r="I116" t="n">
+        <v>45</v>
+      </c>
+      <c r="J116" t="inlineStr">
+        <is>
+          <t>8E1D.jpg</t>
+        </is>
+      </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="L116" t="inlineStr"/>
+      <c r="M116" t="b">
+        <v>0</v>
+      </c>
+      <c r="N116" t="b">
+        <v>0</v>
+      </c>
+      <c r="O116" t="inlineStr"/>
+      <c r="P116" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>646D</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Sainaveen Kothapalli</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr"/>
+      <c r="D117" t="inlineStr"/>
+      <c r="E117" t="inlineStr"/>
+      <c r="F117" t="inlineStr"/>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>All-rounder</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr"/>
+      <c r="I117" t="n">
+        <v>50</v>
+      </c>
+      <c r="J117" t="inlineStr">
+        <is>
+          <t>646D.jpg</t>
+        </is>
+      </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>Sold</t>
+        </is>
+      </c>
+      <c r="L117" t="inlineStr"/>
+      <c r="M117" t="b">
+        <v>0</v>
+      </c>
+      <c r="N117" t="b">
+        <v>1</v>
+      </c>
+      <c r="O117" t="inlineStr">
+        <is>
+          <t>Team 8</t>
+        </is>
+      </c>
+      <c r="P117" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>3H3Y</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Surya Kiran Aravelli</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr"/>
+      <c r="D118" t="inlineStr"/>
+      <c r="E118" t="inlineStr"/>
+      <c r="F118" t="inlineStr"/>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>All-rounder</t>
+        </is>
+      </c>
+      <c r="H118" t="inlineStr"/>
+      <c r="I118" t="n">
+        <v>50</v>
+      </c>
+      <c r="J118" t="inlineStr">
+        <is>
+          <t>3H3Y.jpg</t>
+        </is>
+      </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>Sold</t>
+        </is>
+      </c>
+      <c r="L118" t="inlineStr"/>
+      <c r="M118" t="b">
+        <v>1</v>
+      </c>
+      <c r="N118" t="b">
+        <v>0</v>
+      </c>
+      <c r="O118" t="inlineStr">
+        <is>
+          <t>Team 3</t>
+        </is>
+      </c>
+      <c r="P118" t="n">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L95"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -5580,24 +7582,24 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.45"/>
   <cols>
-    <col width="19.88671875" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="77.44140625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="19.85546875" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="77.42578125" bestFit="1" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Step</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Action</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>Details</t>
         </is>
@@ -5710,25 +7712,25 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.45"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Field</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>AllowedValue</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>UsedFor</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Important</t>
         </is>
@@ -5927,29 +7929,29 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="15.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="15.42578125" defaultRowHeight="14.45"/>
   <cols>
-    <col width="17.88671875" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="44.33203125" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="17.85546875" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="44.28515625" bestFit="1" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Role</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Tier</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>TokenRange</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
@@ -6324,30 +8326,30 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.45"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Role</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Count</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>CurrentAvgTokens</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>RecommendedRange</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>

</xml_diff>

<commit_message>
Update Excel files with latest player and captain data - Add Teams sheet to CPL_Players_Editable.xlsx - Update captain assignments with all 8 captains and vice-captains - Add quality_strikers.png image
</commit_message>
<xml_diff>
--- a/data/CPL_Players_Editable.xlsx
+++ b/data/CPL_Players_Editable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12504" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12504"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="1" r:id="rId1"/>
@@ -1276,9 +1276,6 @@
     <t>CPL_T05</t>
   </si>
   <si>
-    <t>team5_logo.png</t>
-  </si>
-  <si>
     <t>CPL_T06</t>
   </si>
   <si>
@@ -1298,6 +1295,9 @@
   </si>
   <si>
     <t>Quality Strikers</t>
+  </si>
+  <si>
+    <t>quality_strikers.png</t>
   </si>
 </sst>
 </file>
@@ -1662,8 +1662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P118"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="O107" sqref="O107"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R112" sqref="R112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5779,7 +5779,7 @@
         <v>346</v>
       </c>
       <c r="M101" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N101" t="b">
         <v>0</v>
@@ -6096,7 +6096,7 @@
         <v>346</v>
       </c>
       <c r="M111" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N111" t="b">
         <v>0</v>
@@ -6338,15 +6338,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -6409,43 +6409,43 @@
         <v>417</v>
       </c>
       <c r="B6" t="s">
+        <v>424</v>
+      </c>
+      <c r="C6" t="s">
         <v>425</v>
-      </c>
-      <c r="C6" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B7" t="s">
         <v>355</v>
       </c>
       <c r="C7" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B8" t="s">
         <v>359</v>
       </c>
       <c r="C8" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B9" t="s">
         <v>386</v>
       </c>
       <c r="C9" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add 2 new players: DYL7 (Ajay Mannepalli) and CNC0 (Venkata Ramana) - Total players now: 119 (103 for auction + 16 pre-assigned)
</commit_message>
<xml_diff>
--- a/data/CPL_Players_Editable.xlsx
+++ b/data/CPL_Players_Editable.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="439">
   <si>
     <t>PlayerID</t>
   </si>
@@ -1252,52 +1252,91 @@
     <t>CPL_T01</t>
   </si>
   <si>
-    <t>team1_logo.png</t>
-  </si>
-  <si>
     <t>CPL_T02</t>
   </si>
   <si>
-    <t>team2_logo.png</t>
-  </si>
-  <si>
     <t>CPL_T03</t>
   </si>
   <si>
-    <t>team3_logo.png</t>
-  </si>
-  <si>
     <t>CPL_T04</t>
   </si>
   <si>
-    <t>team4_logo.png</t>
-  </si>
-  <si>
     <t>CPL_T05</t>
   </si>
   <si>
     <t>CPL_T06</t>
   </si>
   <si>
-    <t>team6_logo.png</t>
-  </si>
-  <si>
     <t>CPL_T07</t>
   </si>
   <si>
-    <t>team7_logo.png</t>
-  </si>
-  <si>
     <t>CPL_T08</t>
   </si>
   <si>
-    <t>team8_logo.png</t>
-  </si>
-  <si>
     <t>Quality Strikers</t>
   </si>
   <si>
-    <t>quality_strikers.png</t>
+    <t>Colruyt Super Kings</t>
+  </si>
+  <si>
+    <t>csk.png</t>
+  </si>
+  <si>
+    <t>Mavericks</t>
+  </si>
+  <si>
+    <t>Mavericks.png</t>
+  </si>
+  <si>
+    <t>digititans.png</t>
+  </si>
+  <si>
+    <t>Avengers.png</t>
+  </si>
+  <si>
+    <t>Quality Strikers.png</t>
+  </si>
+  <si>
+    <t>Pirates.png</t>
+  </si>
+  <si>
+    <t>Feralessfalcons.png</t>
+  </si>
+  <si>
+    <t>HitsMisses.png</t>
+  </si>
+  <si>
+    <t>Hits &amp; Misses</t>
+  </si>
+  <si>
+    <t>Fearless Falcons</t>
+  </si>
+  <si>
+    <t>Pirates XI</t>
+  </si>
+  <si>
+    <t>Avengers 11</t>
+  </si>
+  <si>
+    <t>Digi Titans</t>
+  </si>
+  <si>
+    <t>DYL7</t>
+  </si>
+  <si>
+    <t>Ajay Mannepalli</t>
+  </si>
+  <si>
+    <t>DYL7.jpg</t>
+  </si>
+  <si>
+    <t>CNC0</t>
+  </si>
+  <si>
+    <t>Venkata Ramana Sashidhar Vasamsetty</t>
+  </si>
+  <si>
+    <t>CNC0.jpg</t>
   </si>
 </sst>
 </file>
@@ -1660,10 +1699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P118"/>
+  <dimension ref="A1:P120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R112" sqref="R112"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A121" sqref="A121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6329,6 +6368,88 @@
         <v>50</v>
       </c>
     </row>
+    <row r="119" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>433</v>
+      </c>
+      <c r="B119" t="s">
+        <v>434</v>
+      </c>
+      <c r="C119" t="s">
+        <v>433</v>
+      </c>
+      <c r="D119">
+        <v>9989056707</v>
+      </c>
+      <c r="E119" t="s">
+        <v>162</v>
+      </c>
+      <c r="F119" t="s">
+        <v>18</v>
+      </c>
+      <c r="G119" t="s">
+        <v>148</v>
+      </c>
+      <c r="H119" t="s">
+        <v>148</v>
+      </c>
+      <c r="I119">
+        <v>40</v>
+      </c>
+      <c r="J119" t="s">
+        <v>435</v>
+      </c>
+      <c r="K119" t="s">
+        <v>22</v>
+      </c>
+      <c r="M119" t="b">
+        <v>0</v>
+      </c>
+      <c r="N119" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>436</v>
+      </c>
+      <c r="B120" t="s">
+        <v>437</v>
+      </c>
+      <c r="C120" t="s">
+        <v>436</v>
+      </c>
+      <c r="D120">
+        <v>9573639955</v>
+      </c>
+      <c r="E120" t="s">
+        <v>162</v>
+      </c>
+      <c r="F120" t="s">
+        <v>18</v>
+      </c>
+      <c r="G120" t="s">
+        <v>148</v>
+      </c>
+      <c r="H120" t="s">
+        <v>148</v>
+      </c>
+      <c r="I120">
+        <v>40</v>
+      </c>
+      <c r="J120" t="s">
+        <v>438</v>
+      </c>
+      <c r="K120" t="s">
+        <v>22</v>
+      </c>
+      <c r="M120" t="b">
+        <v>0</v>
+      </c>
+      <c r="N120" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -6339,13 +6460,13 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
     <col min="3" max="3" width="31.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6365,87 +6486,87 @@
         <v>409</v>
       </c>
       <c r="B2" t="s">
-        <v>347</v>
+        <v>418</v>
       </c>
       <c r="C2" t="s">
-        <v>410</v>
+        <v>419</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B3" t="s">
-        <v>376</v>
+        <v>420</v>
       </c>
       <c r="C3" t="s">
-        <v>412</v>
+        <v>421</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B4" t="s">
-        <v>390</v>
+        <v>432</v>
       </c>
       <c r="C4" t="s">
-        <v>414</v>
+        <v>422</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="B5" t="s">
-        <v>366</v>
+        <v>431</v>
       </c>
       <c r="C5" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>413</v>
+      </c>
+      <c r="B6" t="s">
         <v>417</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>424</v>
-      </c>
-      <c r="C6" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B7" t="s">
-        <v>355</v>
+        <v>430</v>
       </c>
       <c r="C7" t="s">
-        <v>419</v>
+        <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="B8" t="s">
-        <v>359</v>
+        <v>429</v>
       </c>
       <c r="C8" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="B9" t="s">
-        <v>386</v>
+        <v>428</v>
       </c>
       <c r="C9" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update team logos and add 2 new players - Replace old team logos with new branded logos (Avengers, Fearless Falcons, etc.) - Add DYL7 (Ajay Mannepalli) and CNC0 (Venkata Ramana) - Total: 119 players (103 for auction + 16 pre-assigned)
</commit_message>
<xml_diff>
--- a/data/CPL_Players_Editable.xlsx
+++ b/data/CPL_Players_Editable.xlsx
@@ -1701,8 +1701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A121" sqref="A121"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="J123" sqref="J123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update team logos and Excel file with latest changes - Updated team logo images (Avengers, Mavericks, Pirates, Digititans) - Removed 'Quality Strikers.png' (replaced with quality_strikers.png) - Updated Excel file with latest player and team data - Add team names and logos update script
</commit_message>
<xml_diff>
--- a/data/CPL_Players_Editable.xlsx
+++ b/data/CPL_Players_Editable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12504"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12504" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="1" r:id="rId1"/>
@@ -1294,9 +1294,6 @@
     <t>Avengers.png</t>
   </si>
   <si>
-    <t>Quality Strikers.png</t>
-  </si>
-  <si>
     <t>Pirates.png</t>
   </si>
   <si>
@@ -1337,6 +1334,9 @@
   </si>
   <si>
     <t>CNC0.jpg</t>
+  </si>
+  <si>
+    <t>quality_strikers.png</t>
   </si>
 </sst>
 </file>
@@ -1701,7 +1701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+    <sheetView topLeftCell="A91" workbookViewId="0">
       <selection activeCell="J123" sqref="J123"/>
     </sheetView>
   </sheetViews>
@@ -6370,13 +6370,13 @@
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
+        <v>432</v>
+      </c>
+      <c r="B119" t="s">
         <v>433</v>
       </c>
-      <c r="B119" t="s">
-        <v>434</v>
-      </c>
       <c r="C119" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D119">
         <v>9989056707</v>
@@ -6397,7 +6397,7 @@
         <v>40</v>
       </c>
       <c r="J119" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K119" t="s">
         <v>22</v>
@@ -6411,13 +6411,13 @@
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
+        <v>435</v>
+      </c>
+      <c r="B120" t="s">
         <v>436</v>
       </c>
-      <c r="B120" t="s">
-        <v>437</v>
-      </c>
       <c r="C120" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D120">
         <v>9573639955</v>
@@ -6438,7 +6438,7 @@
         <v>40</v>
       </c>
       <c r="J120" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="K120" t="s">
         <v>22</v>
@@ -6459,8 +6459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6508,7 +6508,7 @@
         <v>411</v>
       </c>
       <c r="B4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C4" t="s">
         <v>422</v>
@@ -6519,7 +6519,7 @@
         <v>412</v>
       </c>
       <c r="B5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C5" t="s">
         <v>423</v>
@@ -6533,7 +6533,7 @@
         <v>417</v>
       </c>
       <c r="C6" t="s">
-        <v>424</v>
+        <v>438</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -6541,10 +6541,10 @@
         <v>414</v>
       </c>
       <c r="B7" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C7" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -6552,10 +6552,10 @@
         <v>415</v>
       </c>
       <c r="B8" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C8" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -6563,10 +6563,10 @@
         <v>416</v>
       </c>
       <c r="B9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
   </sheetData>

</xml_diff>